<commit_message>
Implement Add Permissions for SNS. Begin work on Phone Number class for SNS for opting in, listing numbers, etc.
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - Core.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - Core.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Code</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>The requested URL's length exceeds the capacity limit for this server.</t>
+  </si>
+  <si>
+    <t>ValidationError - The input fails to satisfy the constraints specified by an AWS service.</t>
+  </si>
+  <si>
+    <t>InvalidParameter - A request parameter does not comply with the associated constraints.</t>
   </si>
 </sst>
 </file>
@@ -510,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,6 +832,22 @@
         <v>38</v>
       </c>
     </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>412037</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>412038</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fill in more gaps in SNS API
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - Core.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - Core.xlsx
@@ -134,9 +134,6 @@
     <t>TemporaryRedirect - A temporary redirect URL was used while DNS values are updated.</t>
   </si>
   <si>
-    <t>Throttling - The connection is currently being throttled.</t>
-  </si>
-  <si>
     <t>Invalid string value.</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>InvalidParameter - A request parameter does not comply with the associated constraints.</t>
+  </si>
+  <si>
+    <t>Throttling/Throttled - The connection is currently being throttled because the rate at which requests have been submitted for this action exceeds the limit for your account.</t>
   </si>
 </sst>
 </file>
@@ -518,14 +518,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="151.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="157.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -813,7 +813,7 @@
         <v>412034</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -821,7 +821,7 @@
         <v>412035</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>412036</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -837,7 +837,7 @@
         <v>412037</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
         <v>412038</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial work on IoT. Create Thing.vi is implemented.
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - Core.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - Core.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Code</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Throttling/Throttled - The connection is currently being throttled because the rate at which requests have been submitted for this action exceeds the limit for your account.</t>
+  </si>
+  <si>
+    <t>SerializationException - An error occurred during serialization. This is probably due to a JSON payload being malformed.</t>
   </si>
 </sst>
 </file>
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,6 +851,14 @@
         <v>39</v>
       </c>
     </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>412039</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>